<commit_message>
updated sample due to change in code
</commit_message>
<xml_diff>
--- a/sample/sample1.xlsx
+++ b/sample/sample1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehar\Documents\projects\marking-script\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17B218-7178-4418-8675-A83D85C3144F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD2C629-4E95-4561-BCFE-C7BD532046B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{BB68460D-1682-4943-85C8-9F5D3F5160BC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BB68460D-1682-4943-85C8-9F5D3F5160BC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Student 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Student 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Student 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Rubric" sheetId="5" r:id="rId1"/>
+    <sheet name="Student 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Student 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Student 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
   <si>
     <t>Questions</t>
   </si>
@@ -461,6 +462,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E3366A-17B9-42AA-9D9B-AE67F84E3AFF}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="42.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
+        <f>SUM(B4:B9)</f>
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(C4:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2">
+        <f>SUM(B14:B15)</f>
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <f>SUM(C14:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C4:C19)</f>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A5890C-C765-4899-8701-EE5D58F4CCD5}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -633,11 +777,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AE3B90-1C6F-490B-BEE7-AA83947636DC}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
+    <sheetView zoomScale="124" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -806,7 +950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A436C6F2-4965-4EA0-9B56-84FA345999D2}">
   <dimension ref="A1:D22"/>
   <sheetViews>

</xml_diff>